<commit_message>
nieuwe versie excel-bestand, bron wordt nu meegegeven
</commit_message>
<xml_diff>
--- a/catalogusdata/Kenniskluis/Regressietest/xls/Uploadcontrole.xlsx
+++ b/catalogusdata/Kenniskluis/Regressietest/xls/Uploadcontrole.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" tabRatio="744" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9576" tabRatio="744"/>
   </bookViews>
   <sheets>
     <sheet name="URI schema" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="149">
   <si>
     <t>tabblad</t>
   </si>
@@ -38,15 +38,9 @@
     <t>uri schema</t>
   </si>
   <si>
-    <t>Concept</t>
-  </si>
-  <si>
     <t>URI schema</t>
   </si>
   <si>
-    <t>http://www.w3.org/2004/02/skos/core#{klasse}</t>
-  </si>
-  <si>
     <t>vocabulaire</t>
   </si>
   <si>
@@ -218,9 +212,6 @@
     <t>collectie</t>
   </si>
   <si>
-    <t>Collection</t>
-  </si>
-  <si>
     <t>Lid</t>
   </si>
   <si>
@@ -245,9 +236,6 @@
     <t>subklasse</t>
   </si>
   <si>
-    <t>Text</t>
-  </si>
-  <si>
     <t>http://purl.org/dc/dcmitype/{subklasse}</t>
   </si>
   <si>
@@ -380,18 +368,12 @@
     <t>zie ook</t>
   </si>
   <si>
-    <t>Kadaster</t>
-  </si>
-  <si>
     <t>Gevalideerd</t>
   </si>
   <si>
     <t>relatedMatch</t>
   </si>
   <si>
-    <t>http://www.kadaster.nl</t>
-  </si>
-  <si>
     <t>http://{source}</t>
   </si>
   <si>
@@ -468,6 +450,27 @@
   </si>
   <si>
     <t>rendier</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>www.google.nl</t>
+  </si>
+  <si>
+    <t>http://{klasse}</t>
+  </si>
+  <si>
+    <t>www.w3.org/2004/02/skos/core#Concept</t>
+  </si>
+  <si>
+    <t>www.w3.org/2004/02/skos/core#Collection</t>
+  </si>
+  <si>
+    <t>purl.org/dc/dcmitype/Text</t>
+  </si>
+  <si>
+    <t>http://pdok-ld-gck.in.kadaster.nl/id/document/{bron}</t>
   </si>
 </sst>
 </file>
@@ -906,8 +909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -933,390 +936,390 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
+        <v>24</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>145</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>146</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C25" t="s">
-        <v>64</v>
+        <v>146</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>4</v>
+        <v>147</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E30" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.3">
@@ -1369,7 +1372,7 @@
     <hyperlink ref="D5" r:id="rId1"/>
     <hyperlink ref="D6" r:id="rId2" location="{eigenschap}"/>
     <hyperlink ref="D7" r:id="rId3" location="{eigenschap}"/>
-    <hyperlink ref="D2" r:id="rId4" location="{klasse}"/>
+    <hyperlink ref="D2" r:id="rId4" location="{klasse}" display="http://www.w3.org/2004/02/skos/core#{klasse}"/>
     <hyperlink ref="D8" r:id="rId5"/>
     <hyperlink ref="D28" r:id="rId6"/>
     <hyperlink ref="D30" r:id="rId7" location="{eigenschap}"/>
@@ -1378,9 +1381,11 @@
     <hyperlink ref="D11" r:id="rId10"/>
     <hyperlink ref="D10" r:id="rId11"/>
     <hyperlink ref="D32" r:id="rId12"/>
+    <hyperlink ref="D3" r:id="rId13" location="{eigenschap}"/>
+    <hyperlink ref="D27" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 
@@ -1388,8 +1393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1410,709 +1415,709 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
         <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
         <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
         <v>34</v>
-      </c>
-      <c r="E10" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
         <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
         <v>43</v>
-      </c>
-      <c r="C12" t="s">
-        <v>87</v>
-      </c>
-      <c r="D12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
         <v>46</v>
-      </c>
-      <c r="C13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" t="s">
         <v>49</v>
-      </c>
-      <c r="C14" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D16" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E16" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E17" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E19" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E20" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" t="s">
         <v>56</v>
-      </c>
-      <c r="C21" t="s">
-        <v>86</v>
-      </c>
-      <c r="D21" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="E23" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>61</v>
       </c>
       <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="D29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="E29" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="E34" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B39" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E39" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E40" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B41" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E41" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -2153,16 +2158,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V8" sqref="V8"/>
+      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="70.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="28.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="28.33203125" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="70.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="70.44140625" style="9" bestFit="1" customWidth="1"/>
@@ -2176,9 +2181,9 @@
     <col min="14" max="14" width="9.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="42.33203125" style="9" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="5.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="32.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9" style="9" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
@@ -2189,204 +2194,209 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="Q1" s="11" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="R1" s="11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="T1" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="U1" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="V1" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="W1" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="V1" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="W1" s="11" t="s">
-        <v>107</v>
-      </c>
       <c r="X1" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="M2" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="N2" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="R2" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="I2" s="9"/>
-      <c r="K2" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="N2" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="R2" s="10" t="s">
-        <v>147</v>
-      </c>
       <c r="V2" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>144</v>
+        <v>138</v>
+      </c>
+      <c r="V3" s="9" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="R4" s="19"/>
       <c r="V4" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="R5" s="20"/>
       <c r="V5" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="V6" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="V7" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="V8" s="9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.3">
@@ -2587,25 +2597,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2664,16 +2674,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -2699,65 +2709,58 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>121</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>142</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>142</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="F2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GCO-131 eerste start aanpassing excel-upload
</commit_message>
<xml_diff>
--- a/catalogusdata/Kenniskluis/Regressietest/xls/Uploadcontrole.xlsx
+++ b/catalogusdata/Kenniskluis/Regressietest/xls/Uploadcontrole.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="150">
   <si>
     <t>tabblad</t>
   </si>
@@ -383,9 +383,6 @@
     <t>http://pdok-ld-gck.in.kadaster.nl/id/concept/{domein}</t>
   </si>
   <si>
-    <t>http://pdok-ld-gck.in.kadaster.nl/id/concept/{bron}</t>
-  </si>
-  <si>
     <t>http://pdok-ld-gck.in.kadaster.nl/id/concept/{specialisatie}</t>
   </si>
   <si>
@@ -471,6 +468,12 @@
   </si>
   <si>
     <t>http://pdok-ld-gck.in.kadaster.nl/id/document/{bron}</t>
+  </si>
+  <si>
+    <t>dc</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/elements/1.1/{eigenschap}</t>
   </si>
 </sst>
 </file>
@@ -910,14 +913,14 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.109375" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" customWidth="1"/>
     <col min="4" max="4" width="72.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -947,7 +950,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1009,10 +1012,10 @@
         <v>6</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>52</v>
+        <v>149</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1023,10 +1026,10 @@
         <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1037,24 +1040,24 @@
         <v>6</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="E8" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" t="s">
-        <v>145</v>
+        <v>6</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>117</v>
+        <v>98</v>
+      </c>
+      <c r="E9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1062,10 +1065,13 @@
         <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
+        <v>144</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1073,10 +1079,10 @@
         <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1084,21 +1090,19 @@
         <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>120</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1106,10 +1110,10 @@
         <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1117,10 +1121,10 @@
         <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1128,10 +1132,10 @@
         <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1139,10 +1143,10 @@
         <v>64</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1150,10 +1154,10 @@
         <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1161,10 +1165,10 @@
         <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1172,10 +1176,10 @@
         <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1183,24 +1187,21 @@
         <v>64</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" t="s">
-        <v>146</v>
+        <v>95</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1208,10 +1209,13 @@
         <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="C23" t="s">
+        <v>145</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1219,24 +1223,21 @@
         <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" t="s">
-        <v>146</v>
+        <v>25</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1244,7 +1245,10 @@
         <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>74</v>
+      </c>
+      <c r="C26" t="s">
+        <v>145</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>130</v>
@@ -1252,16 +1256,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" t="s">
-        <v>147</v>
+        <v>61</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1269,10 +1270,13 @@
         <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>31</v>
+      </c>
+      <c r="C28" t="s">
+        <v>146</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>70</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1280,35 +1284,35 @@
         <v>72</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E30" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>102</v>
+        <v>6</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
+      </c>
+      <c r="E31" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1316,73 +1320,81 @@
         <v>64</v>
       </c>
       <c r="B32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
         <v>112</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D33" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D47" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1"/>
-    <hyperlink ref="D6" r:id="rId2" location="{eigenschap}"/>
-    <hyperlink ref="D7" r:id="rId3" location="{eigenschap}"/>
+    <hyperlink ref="D7" r:id="rId2" location="{eigenschap}"/>
+    <hyperlink ref="D8" r:id="rId3" location="{eigenschap}"/>
     <hyperlink ref="D2" r:id="rId4" location="{klasse}" display="http://www.w3.org/2004/02/skos/core#{klasse}"/>
-    <hyperlink ref="D8" r:id="rId5"/>
-    <hyperlink ref="D28" r:id="rId6"/>
-    <hyperlink ref="D30" r:id="rId7" location="{eigenschap}"/>
-    <hyperlink ref="D31" r:id="rId8"/>
-    <hyperlink ref="D9" r:id="rId9"/>
+    <hyperlink ref="D9" r:id="rId5"/>
+    <hyperlink ref="D29" r:id="rId6"/>
+    <hyperlink ref="D31" r:id="rId7" location="{eigenschap}"/>
+    <hyperlink ref="D32" r:id="rId8"/>
+    <hyperlink ref="D10" r:id="rId9"/>
     <hyperlink ref="D11" r:id="rId10"/>
-    <hyperlink ref="D10" r:id="rId11"/>
-    <hyperlink ref="D32" r:id="rId12"/>
-    <hyperlink ref="D3" r:id="rId13" location="{eigenschap}"/>
-    <hyperlink ref="D27" r:id="rId14"/>
+    <hyperlink ref="D33" r:id="rId11"/>
+    <hyperlink ref="D3" r:id="rId12" location="{eigenschap}"/>
+    <hyperlink ref="D28" r:id="rId13"/>
+    <hyperlink ref="D6" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
@@ -1393,7 +1405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1583,7 +1595,7 @@
         <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>82</v>
+        <v>148</v>
       </c>
       <c r="D10" t="s">
         <v>32</v>
@@ -2268,43 +2280,43 @@
     </row>
     <row r="2" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="I2" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="K2" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="K2" s="10" t="s">
+      <c r="L2" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="M2" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="L2" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="M2" s="10" t="s">
+      <c r="N2" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="R2" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="R2" s="10" t="s">
-        <v>141</v>
       </c>
       <c r="V2" s="9" t="s">
         <v>114</v>
@@ -2312,16 +2324,16 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="V3" s="9" t="s">
         <v>114</v>
@@ -2329,13 +2341,13 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R4" s="19"/>
       <c r="V4" s="9" t="s">
@@ -2344,13 +2356,13 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="R5" s="20"/>
       <c r="V5" s="9" t="s">
@@ -2359,13 +2371,13 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="V6" s="9" t="s">
         <v>114</v>
@@ -2373,13 +2385,13 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="V7" s="9" t="s">
         <v>114</v>
@@ -2387,13 +2399,13 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="V8" s="9" t="s">
         <v>114</v>
@@ -2712,7 +2724,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2743,16 +2755,16 @@
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="B2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
GCO-131 excel-upload bronnen aanpassen
</commit_message>
<xml_diff>
--- a/catalogusdata/Kenniskluis/Regressietest/xls/Uploadcontrole.xlsx
+++ b/catalogusdata/Kenniskluis/Regressietest/xls/Uploadcontrole.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9576" tabRatio="744"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9576" tabRatio="744" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="URI schema" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="154">
   <si>
     <t>tabblad</t>
   </si>
@@ -474,6 +474,18 @@
   </si>
   <si>
     <t>http://purl.org/dc/elements/1.1/{eigenschap}</t>
+  </si>
+  <si>
+    <t>tekst</t>
+  </si>
+  <si>
+    <t>dit zijn poten.</t>
+  </si>
+  <si>
+    <t>literal</t>
+  </si>
+  <si>
+    <t>tekstbron</t>
   </si>
 </sst>
 </file>
@@ -912,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1092,7 +1104,9 @@
       <c r="B12" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1338,6 +1352,12 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" t="s">
+        <v>153</v>
+      </c>
       <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1395,9 +1415,10 @@
     <hyperlink ref="D3" r:id="rId12" location="{eigenschap}"/>
     <hyperlink ref="D28" r:id="rId13"/>
     <hyperlink ref="D6" r:id="rId14"/>
+    <hyperlink ref="D12" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 
@@ -1405,8 +1426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2132,6 +2153,23 @@
         <v>108</v>
       </c>
     </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
@@ -2168,13 +2206,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X80"/>
+  <dimension ref="A1:Y80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="70.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2183,28 +2221,29 @@
     <col min="4" max="4" width="70.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.44140625" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="70.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="89.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.5546875" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="42.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="32.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9" style="9" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="70.5546875" style="9"/>
+    <col min="9" max="9" width="9.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="42.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="32.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9" style="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="70.5546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>63</v>
       </c>
@@ -2230,55 +2269,58 @@
         <v>35</v>
       </c>
       <c r="I1" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="R1" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="S1" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="T1" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="U1" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="V1" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="W1" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="X1" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="Y1" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>132</v>
       </c>
@@ -2300,29 +2342,29 @@
       <c r="H2" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="L2" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="M2" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="N2" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="O2" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="S2" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="W2" s="9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>132</v>
       </c>
@@ -2332,14 +2374,14 @@
       <c r="C3" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="S3" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="V3" s="9" t="s">
+      <c r="W3" s="9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>136</v>
       </c>
@@ -2349,12 +2391,12 @@
       <c r="C4" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="R4" s="19"/>
-      <c r="V4" s="9" t="s">
+      <c r="S4" s="19"/>
+      <c r="W4" s="9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>137</v>
       </c>
@@ -2364,12 +2406,12 @@
       <c r="C5" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="R5" s="20"/>
-      <c r="V5" s="9" t="s">
+      <c r="S5" s="20"/>
+      <c r="W5" s="9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>138</v>
       </c>
@@ -2379,11 +2421,11 @@
       <c r="C6" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="V6" s="9" t="s">
+      <c r="W6" s="9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>139</v>
       </c>
@@ -2393,11 +2435,17 @@
       <c r="C7" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="V7" s="9" t="s">
+      <c r="D7" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="W7" s="9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>140</v>
       </c>
@@ -2407,17 +2455,16 @@
       <c r="C8" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="V8" s="9" t="s">
+      <c r="W8" s="9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="P21" s="10"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="10"/>
+      <c r="N21" s="10"/>
       <c r="Q21" s="10"/>
       <c r="R21" s="10"/>
       <c r="S21" s="10"/>
@@ -2426,81 +2473,82 @@
       <c r="V21" s="10"/>
       <c r="W21" s="10"/>
       <c r="X21" s="10"/>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="Y21" s="10"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G24" s="10"/>
     </row>
-    <row r="25" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G25" s="10"/>
-      <c r="J25" s="12"/>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="K25" s="12"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="G26" s="10"/>
-      <c r="J26" s="12"/>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="K26" s="12"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
       <c r="G27" s="10"/>
-      <c r="J27" s="12"/>
-    </row>
-    <row r="28" spans="1:24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K27" s="12"/>
+    </row>
+    <row r="28" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
       <c r="G28" s="10"/>
-      <c r="J28" s="12"/>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="K28" s="12"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
       <c r="G29" s="10"/>
-      <c r="J29" s="12"/>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="K29" s="12"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="G30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="15"/>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="J30" s="10"/>
+      <c r="K30" s="15"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="10"/>
-      <c r="M31" s="10"/>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="K31" s="12"/>
+      <c r="L31" s="10"/>
+      <c r="N31" s="10"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="10"/>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="O32" s="10"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K32" s="12"/>
+      <c r="L32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="P32" s="10"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
       <c r="C33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="10"/>
-      <c r="M33" s="10"/>
-      <c r="O33" s="10"/>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K33" s="12"/>
+      <c r="L33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="P33" s="10"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
       <c r="C34" s="10"/>
@@ -2508,73 +2556,73 @@
       <c r="F34" s="17"/>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="10"/>
-      <c r="M34" s="10"/>
-      <c r="O34" s="14"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K34" s="12"/>
+      <c r="L34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="P34" s="14"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E35" s="17"/>
       <c r="F35" s="17"/>
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="10"/>
-      <c r="M35" s="10"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K35" s="12"/>
+      <c r="L35" s="10"/>
+      <c r="N35" s="10"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E36" s="17"/>
       <c r="F36" s="17"/>
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="10"/>
-      <c r="M36" s="10"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K36" s="12"/>
+      <c r="L36" s="10"/>
+      <c r="N36" s="10"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E37" s="17"/>
       <c r="F37" s="17"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
       <c r="G38" s="10"/>
       <c r="H38" s="10"/>
-      <c r="J38" s="12"/>
-      <c r="K38" s="10"/>
-      <c r="M38" s="10"/>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K38" s="12"/>
+      <c r="L38" s="10"/>
+      <c r="N38" s="10"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E39" s="17"/>
       <c r="F39" s="17"/>
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>
-      <c r="J39" s="12"/>
-      <c r="K39" s="10"/>
-      <c r="M39" s="10"/>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K39" s="12"/>
+      <c r="L39" s="10"/>
+      <c r="N39" s="10"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E40" s="17"/>
       <c r="F40" s="17"/>
       <c r="G40" s="10"/>
       <c r="H40" s="10"/>
-      <c r="J40" s="12"/>
-      <c r="K40" s="10"/>
-      <c r="M40" s="10"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="K40" s="12"/>
+      <c r="L40" s="10"/>
+      <c r="N40" s="10"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E41" s="17"/>
       <c r="F41" s="17"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>
     </row>
@@ -2724,7 +2772,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E6" sqref="A2:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>